<commit_message>
feat: migrate full SGV platform to Symfony 6.4
- Complete migration from legacy DashboardBundle to Symfony 6.4
- EasyAdmin 4.x dashboards (Admin, COT, SIV)
- WhatsApp Business API integration (Meta Cloud API)
- Prometheus/Grafana/Alertmanager monitoring stack
- OPC Daemon polling migration with bulk UPDATE optimization
- JWT + OAuth2 authentication with 2FA support
- Webhook processing via Symfony Messenger async queue
- Security hardening: secrets moved to env vars, .gitignore hardened
- docs/ excluded from repo (contains local credentials and legacy code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/files/templates/lista_acumulado_atencion_incidentes_por_clase_vehiculo - copia.xlsx
+++ b/public/files/templates/lista_acumulado_atencion_incidentes_por_clase_vehiculo - copia.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\source\repos\server\vs.gvops.cl\public\files\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA8F03D-0C69-4AE4-B139-4D0E7351C854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -353,22 +359,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -381,10 +372,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -399,7 +390,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -431,7 +422,13 @@
     <xdr:ext cx="1428750" cy="542925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Logo" descr="Logo"/>
+        <xdr:cNvPr id="2" name="Logo" descr="Logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -446,39 +443,6 @@
         <a:xfrm>
           <a:off x="72471" y="124236"/>
           <a:ext cx="1428750" cy="542925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>289672</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1247775" cy="828675"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Logo" descr="Logo"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12548907" y="22412"/>
-          <a:ext cx="1247775" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -745,80 +709,79 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1" style="16" customWidth="1"/>
+    <col min="1" max="1" width="1" style="15" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="7" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" style="7" customWidth="1"/>
-    <col min="8" max="18" width="7.7109375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="15" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" style="24" customWidth="1"/>
+    <col min="8" max="19" width="7.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" style="19" customWidth="1"/>
     <col min="21" max="50" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -870,25 +833,25 @@
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="20"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -907,10 +870,10 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="29"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
       <c r="T6" s="14"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -936,37 +899,37 @@
       <c r="T7" s="13"/>
     </row>
     <row r="8" spans="1:20" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="25"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>